<commit_message>
Update sample 15C BOM.
</commit_message>
<xml_diff>
--- a/15C-Red-BOM-2015-11-04.xlsx
+++ b/15C-Red-BOM-2015-11-04.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="700" windowWidth="25600" windowHeight="17540"/>
+    <workbookView xWindow="-25600" yWindow="460" windowWidth="25600" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="UX Package Info" sheetId="5" r:id="rId1"/>
@@ -588,9 +588,6 @@
     <t>BE3-R (NIC, iSCSI, FCoE)</t>
   </si>
   <si>
-    <t>Lancer (FC)</t>
-  </si>
-  <si>
     <t>Saturn (FC)</t>
   </si>
   <si>
@@ -1169,6 +1166,9 @@
   </si>
   <si>
     <t>Added PLDM FW Download Data column (column M) and specified necessary data for all applicable adapters</t>
+  </si>
+  <si>
+    <t>Lancer G5 (FC)</t>
   </si>
 </sst>
 </file>
@@ -1613,7 +1613,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1894,8 +1894,17 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1951,18 +1960,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="204">
@@ -2494,38 +2491,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
-        <v>310</v>
-      </c>
-      <c r="B1" s="107"/>
+      <c r="A1" s="110" t="s">
+        <v>309</v>
+      </c>
+      <c r="B1" s="110"/>
       <c r="C1" s="100"/>
       <c r="D1" s="100"/>
     </row>
     <row r="2" spans="1:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="107" t="s">
-        <v>311</v>
-      </c>
-      <c r="B2" s="107"/>
+      <c r="A2" s="110" t="s">
+        <v>310</v>
+      </c>
+      <c r="B2" s="110"/>
     </row>
     <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="12"/>
-      <c r="D4" s="129" t="s">
-        <v>314</v>
-      </c>
-      <c r="E4" s="129"/>
-      <c r="F4" s="129"/>
+      <c r="D4" s="109" t="s">
+        <v>313</v>
+      </c>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="129" t="s">
+      <c r="H4" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="129"/>
-      <c r="J4" s="129"/>
-      <c r="K4" s="129"/>
-      <c r="L4" s="129"/>
-      <c r="M4" s="129"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="109"/>
+      <c r="K4" s="109"/>
+      <c r="L4" s="109"/>
+      <c r="M4" s="109"/>
       <c r="N4" s="14"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -2559,7 +2556,7 @@
         <v>36</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="N5" s="20"/>
     </row>
@@ -2568,27 +2565,27 @@
         <v>32</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="126" t="s">
+      <c r="D6" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="127"/>
-      <c r="F6" s="128"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="108"/>
       <c r="G6" s="21"/>
-      <c r="H6" s="126" t="s">
+      <c r="H6" s="106" t="s">
         <v>175</v>
       </c>
-      <c r="I6" s="127"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
-      <c r="L6" s="128"/>
-      <c r="M6" s="106"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="107"/>
+      <c r="L6" s="107"/>
+      <c r="M6" s="108"/>
       <c r="N6" s="22"/>
       <c r="O6" s="72"/>
       <c r="P6" s="23"/>
     </row>
     <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.2">
       <c r="B7" s="81" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="25" t="s">
@@ -2602,7 +2599,7 @@
       </c>
       <c r="G7" s="28"/>
       <c r="H7" s="88" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I7" s="86" t="s">
         <v>145</v>
@@ -2617,7 +2614,7 @@
         <v>42</v>
       </c>
       <c r="M7" s="76" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N7" s="22"/>
       <c r="O7" s="72"/>
@@ -2625,7 +2622,7 @@
     </row>
     <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.2">
       <c r="B8" s="81" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="29" t="s">
@@ -2639,29 +2636,29 @@
       </c>
       <c r="G8" s="33"/>
       <c r="H8" s="88" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I8" s="39" t="s">
+        <v>212</v>
+      </c>
+      <c r="J8" s="39" t="s">
         <v>213</v>
       </c>
-      <c r="J8" s="39" t="s">
+      <c r="K8" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="K8" s="38" t="s">
+      <c r="L8" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="L8" s="38" t="s">
-        <v>216</v>
-      </c>
       <c r="M8" s="76" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O8" s="72"/>
       <c r="P8" s="30"/>
     </row>
     <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.2">
       <c r="B9" s="83" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="25" t="s">
@@ -2675,29 +2672,29 @@
       </c>
       <c r="G9" s="33"/>
       <c r="H9" s="101" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I9" s="39" t="s">
+        <v>216</v>
+      </c>
+      <c r="J9" s="39" t="s">
         <v>217</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="K9" s="39" t="s">
+        <v>217</v>
+      </c>
+      <c r="L9" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="K9" s="39" t="s">
-        <v>218</v>
-      </c>
-      <c r="L9" s="38" t="s">
-        <v>219</v>
-      </c>
       <c r="M9" s="76" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O9" s="72"/>
       <c r="P9" s="30"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B10" s="81" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C10" s="34"/>
       <c r="D10" s="15" t="s">
@@ -2715,7 +2712,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="83" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C11" s="34"/>
       <c r="D11" s="25" t="s">
@@ -2728,24 +2725,24 @@
         <v>5</v>
       </c>
       <c r="G11" s="37"/>
-      <c r="H11" s="125" t="s">
-        <v>176</v>
-      </c>
-      <c r="I11" s="125"/>
-      <c r="J11" s="125"/>
-      <c r="K11" s="125"/>
-      <c r="L11" s="125"/>
-      <c r="M11" s="125"/>
+      <c r="H11" s="128" t="s">
+        <v>358</v>
+      </c>
+      <c r="I11" s="128"/>
+      <c r="J11" s="128"/>
+      <c r="K11" s="128"/>
+      <c r="L11" s="128"/>
+      <c r="M11" s="128"/>
       <c r="O11" s="72"/>
       <c r="P11" s="30"/>
     </row>
     <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.2">
       <c r="B12" s="81" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C12" s="34"/>
       <c r="D12" s="25" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E12" s="35">
         <v>5467</v>
@@ -2754,8 +2751,8 @@
         <v>6</v>
       </c>
       <c r="G12" s="28"/>
-      <c r="H12" s="110" t="s">
-        <v>345</v>
+      <c r="H12" s="113" t="s">
+        <v>344</v>
       </c>
       <c r="I12" s="86" t="s">
         <v>150</v>
@@ -2770,18 +2767,18 @@
         <v>153</v>
       </c>
       <c r="M12" s="86" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="O12" s="72"/>
       <c r="P12" s="30"/>
     </row>
     <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.2">
       <c r="B13" s="81" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C13" s="34"/>
       <c r="D13" s="39" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E13" s="35">
         <v>8753</v>
@@ -2790,7 +2787,7 @@
         <v>7</v>
       </c>
       <c r="G13" s="28"/>
-      <c r="H13" s="116"/>
+      <c r="H13" s="119"/>
       <c r="I13" s="86" t="s">
         <v>154</v>
       </c>
@@ -2804,18 +2801,18 @@
         <v>157</v>
       </c>
       <c r="M13" s="86" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="O13" s="72"/>
       <c r="P13" s="30"/>
     </row>
     <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.2">
       <c r="B14" s="81" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C14" s="41"/>
       <c r="D14" s="29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E14" s="31">
         <v>8869</v>
@@ -2823,7 +2820,7 @@
       <c r="F14" s="32">
         <v>8</v>
       </c>
-      <c r="H14" s="116"/>
+      <c r="H14" s="119"/>
       <c r="I14" s="95" t="s">
         <v>158</v>
       </c>
@@ -2837,18 +2834,18 @@
         <v>153</v>
       </c>
       <c r="M14" s="86" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="O14" s="72"/>
       <c r="P14" s="30"/>
     </row>
     <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.2">
       <c r="B15" s="83" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C15" s="41"/>
       <c r="D15" s="25" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E15" s="35">
         <v>8871</v>
@@ -2856,7 +2853,7 @@
       <c r="F15" s="27">
         <v>9</v>
       </c>
-      <c r="H15" s="111"/>
+      <c r="H15" s="114"/>
       <c r="I15" s="86" t="s">
         <v>160</v>
       </c>
@@ -2864,155 +2861,155 @@
         <v>155</v>
       </c>
       <c r="K15" s="86" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L15" s="86" t="s">
         <v>157</v>
       </c>
       <c r="M15" s="86" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="O15" s="72"/>
       <c r="P15" s="30"/>
     </row>
     <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.2">
       <c r="B16" s="83" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C16" s="41"/>
       <c r="D16" s="25" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F16" s="27">
         <v>10</v>
       </c>
-      <c r="H16" s="110" t="s">
-        <v>319</v>
+      <c r="H16" s="113" t="s">
+        <v>318</v>
       </c>
       <c r="I16" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="J16" s="87" t="s">
         <v>220</v>
       </c>
-      <c r="J16" s="87" t="s">
+      <c r="K16" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="K16" s="38" t="s">
+      <c r="L16" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="L16" s="38" t="s">
-        <v>223</v>
-      </c>
       <c r="M16" s="86" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="O16" s="72"/>
       <c r="P16" s="30"/>
     </row>
     <row r="17" spans="2:16" ht="30" x14ac:dyDescent="0.2">
       <c r="B17" s="82" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C17" s="45"/>
       <c r="D17" s="52"/>
       <c r="E17" s="103"/>
       <c r="F17" s="104"/>
       <c r="G17" s="72"/>
-      <c r="H17" s="111"/>
+      <c r="H17" s="114"/>
       <c r="I17" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="J17" s="87" t="s">
+        <v>220</v>
+      </c>
+      <c r="K17" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="J17" s="87" t="s">
-        <v>221</v>
-      </c>
-      <c r="K17" s="38" t="s">
-        <v>229</v>
-      </c>
       <c r="L17" s="38" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M17" s="86" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="O17" s="72"/>
       <c r="P17" s="30"/>
     </row>
     <row r="18" spans="2:16" ht="30" x14ac:dyDescent="0.2">
       <c r="B18" s="81" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C18" s="8"/>
-      <c r="D18" s="122" t="s">
-        <v>212</v>
-      </c>
-      <c r="E18" s="123"/>
-      <c r="F18" s="124"/>
+      <c r="D18" s="125" t="s">
+        <v>211</v>
+      </c>
+      <c r="E18" s="126"/>
+      <c r="F18" s="127"/>
       <c r="G18" s="72"/>
-      <c r="H18" s="112" t="s">
-        <v>317</v>
+      <c r="H18" s="115" t="s">
+        <v>316</v>
       </c>
       <c r="I18" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="J18" s="39" t="s">
         <v>224</v>
       </c>
-      <c r="J18" s="39" t="s">
+      <c r="K18" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="K18" s="38" t="s">
+      <c r="L18" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="L18" s="38" t="s">
-        <v>227</v>
-      </c>
       <c r="M18" s="86" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="O18" s="72"/>
       <c r="P18" s="30"/>
     </row>
     <row r="19" spans="2:16" ht="30" x14ac:dyDescent="0.2">
       <c r="B19" s="82" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="87" t="s">
+        <v>203</v>
+      </c>
+      <c r="E19" s="75" t="s">
         <v>204</v>
-      </c>
-      <c r="E19" s="75" t="s">
-        <v>205</v>
       </c>
       <c r="F19" s="43">
         <v>50</v>
       </c>
       <c r="G19" s="72"/>
-      <c r="H19" s="113"/>
+      <c r="H19" s="116"/>
       <c r="I19" s="38" t="s">
+        <v>229</v>
+      </c>
+      <c r="J19" s="39" t="s">
+        <v>224</v>
+      </c>
+      <c r="K19" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="J19" s="39" t="s">
-        <v>225</v>
-      </c>
-      <c r="K19" s="38" t="s">
-        <v>231</v>
-      </c>
       <c r="L19" s="38" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M19" s="86" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="O19" s="72"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B20" s="81" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="87" t="s">
+        <v>205</v>
+      </c>
+      <c r="E20" s="42" t="s">
         <v>206</v>
-      </c>
-      <c r="E20" s="42" t="s">
-        <v>207</v>
       </c>
       <c r="F20" s="43">
         <v>51</v>
@@ -3022,44 +3019,44 @@
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B21" s="83" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="87" t="s">
+        <v>207</v>
+      </c>
+      <c r="E21" s="42" t="s">
         <v>208</v>
-      </c>
-      <c r="E21" s="42" t="s">
-        <v>209</v>
       </c>
       <c r="F21" s="76">
         <v>52</v>
       </c>
-      <c r="H21" s="125" t="s">
-        <v>177</v>
-      </c>
-      <c r="I21" s="125"/>
-      <c r="J21" s="125"/>
-      <c r="K21" s="125"/>
-      <c r="L21" s="125"/>
-      <c r="M21" s="125"/>
+      <c r="H21" s="128" t="s">
+        <v>176</v>
+      </c>
+      <c r="I21" s="128"/>
+      <c r="J21" s="128"/>
+      <c r="K21" s="128"/>
+      <c r="L21" s="128"/>
+      <c r="M21" s="128"/>
       <c r="O21" s="72"/>
     </row>
     <row r="22" spans="2:16" ht="45" x14ac:dyDescent="0.2">
       <c r="B22" s="81" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="61" t="s">
+        <v>209</v>
+      </c>
+      <c r="E22" s="42" t="s">
         <v>210</v>
-      </c>
-      <c r="E22" s="42" t="s">
-        <v>211</v>
       </c>
       <c r="F22" s="77">
         <v>53</v>
       </c>
-      <c r="H22" s="114" t="s">
-        <v>345</v>
+      <c r="H22" s="117" t="s">
+        <v>344</v>
       </c>
       <c r="I22" s="86" t="s">
         <v>161</v>
@@ -3074,16 +3071,16 @@
         <v>164</v>
       </c>
       <c r="M22" s="76" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O22" s="72"/>
     </row>
     <row r="23" spans="2:16" ht="45" x14ac:dyDescent="0.2">
       <c r="B23" s="83" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="H23" s="115"/>
+      <c r="H23" s="118"/>
       <c r="I23" s="86" t="s">
         <v>165</v>
       </c>
@@ -3097,38 +3094,38 @@
         <v>164</v>
       </c>
       <c r="M23" s="76" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O23" s="72"/>
     </row>
     <row r="24" spans="2:16" ht="45" x14ac:dyDescent="0.2">
       <c r="B24" s="83" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C24" s="8"/>
       <c r="H24" s="94" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I24" s="39" t="s">
+        <v>231</v>
+      </c>
+      <c r="J24" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="J24" s="39" t="s">
+      <c r="K24" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="K24" s="38" t="s">
+      <c r="L24" s="38" t="s">
         <v>234</v>
       </c>
-      <c r="L24" s="38" t="s">
-        <v>235</v>
-      </c>
       <c r="M24" s="76" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O24" s="72"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="83" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D25" s="44"/>
       <c r="E25" s="7"/>
@@ -3137,29 +3134,29 @@
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B26" s="83" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D26" s="44"/>
       <c r="E26" s="7"/>
       <c r="F26" s="46"/>
-      <c r="H26" s="125" t="s">
-        <v>178</v>
-      </c>
-      <c r="I26" s="125"/>
-      <c r="J26" s="125"/>
-      <c r="K26" s="125"/>
-      <c r="L26" s="125"/>
-      <c r="M26" s="125"/>
+      <c r="H26" s="128" t="s">
+        <v>177</v>
+      </c>
+      <c r="I26" s="128"/>
+      <c r="J26" s="128"/>
+      <c r="K26" s="128"/>
+      <c r="L26" s="128"/>
+      <c r="M26" s="128"/>
       <c r="O26" s="72"/>
     </row>
     <row r="27" spans="2:16" ht="30" x14ac:dyDescent="0.2">
       <c r="B27" s="81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="46"/>
-      <c r="H27" s="117" t="s">
-        <v>263</v>
+      <c r="H27" s="120" t="s">
+        <v>262</v>
       </c>
       <c r="I27" s="86" t="s">
         <v>168</v>
@@ -3174,18 +3171,18 @@
         <v>43</v>
       </c>
       <c r="M27" s="76" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O27" s="72"/>
     </row>
     <row r="28" spans="2:16" ht="30" x14ac:dyDescent="0.2">
       <c r="B28" s="47" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D28" s="67"/>
       <c r="E28" s="64"/>
       <c r="F28" s="68"/>
-      <c r="H28" s="118"/>
+      <c r="H28" s="121"/>
       <c r="I28" s="86" t="s">
         <v>174</v>
       </c>
@@ -3199,18 +3196,18 @@
         <v>44</v>
       </c>
       <c r="M28" s="76" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="O28" s="72"/>
     </row>
     <row r="29" spans="2:16" ht="30" x14ac:dyDescent="0.2">
       <c r="B29" s="83" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D29" s="67"/>
       <c r="E29" s="64"/>
       <c r="F29" s="68"/>
-      <c r="H29" s="119"/>
+      <c r="H29" s="122"/>
       <c r="I29" s="87" t="s">
         <v>45</v>
       </c>
@@ -3218,13 +3215,13 @@
         <v>41</v>
       </c>
       <c r="K29" s="86" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L29" s="86" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M29" s="76" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="30" spans="2:16" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -3232,44 +3229,44 @@
       <c r="D30" s="44"/>
       <c r="E30" s="7"/>
       <c r="F30" s="46"/>
-      <c r="H30" s="120" t="s">
-        <v>345</v>
+      <c r="H30" s="123" t="s">
+        <v>344</v>
       </c>
       <c r="I30" s="87" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J30" s="87" t="s">
         <v>140</v>
       </c>
       <c r="K30" s="86" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L30" s="86" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M30" s="86" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="31" spans="2:16" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="D31" s="44"/>
       <c r="E31" s="7"/>
       <c r="F31" s="46"/>
-      <c r="H31" s="121"/>
+      <c r="H31" s="124"/>
       <c r="I31" s="87" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J31" s="87" t="s">
         <v>141</v>
       </c>
       <c r="K31" s="86" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L31" s="86" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="M31" s="86" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="32" spans="2:16" ht="60" x14ac:dyDescent="0.2">
@@ -3277,7 +3274,7 @@
       <c r="E32" s="7"/>
       <c r="F32" s="46"/>
       <c r="H32" s="102" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I32" s="87" t="s">
         <v>146</v>
@@ -3286,33 +3283,33 @@
         <v>147</v>
       </c>
       <c r="K32" s="86" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L32" s="86" t="s">
         <v>148</v>
       </c>
       <c r="M32" s="76" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="33" spans="4:14" ht="30" x14ac:dyDescent="0.2">
       <c r="H33" s="102" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I33" s="87" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J33" s="87" t="s">
         <v>147</v>
       </c>
       <c r="K33" s="86" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L33" s="86" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M33" s="86" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="N33" s="23"/>
     </row>
@@ -3321,66 +3318,66 @@
       <c r="E34" s="7"/>
       <c r="F34" s="46"/>
       <c r="H34" s="78" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I34" s="39" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J34" s="39" t="s">
+        <v>235</v>
+      </c>
+      <c r="K34" s="38" t="s">
         <v>236</v>
       </c>
-      <c r="K34" s="38" t="s">
+      <c r="L34" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="L34" s="38" t="s">
-        <v>238</v>
-      </c>
       <c r="M34" s="76" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="35" spans="4:14" ht="30" x14ac:dyDescent="0.2">
       <c r="D35" s="44"/>
       <c r="E35" s="7"/>
       <c r="F35" s="46"/>
-      <c r="H35" s="108" t="s">
-        <v>320</v>
+      <c r="H35" s="111" t="s">
+        <v>319</v>
       </c>
       <c r="I35" s="87" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J35" s="85" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K35" s="85" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L35" s="89" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="M35" s="86" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="36" spans="4:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D36" s="48"/>
       <c r="E36" s="6"/>
       <c r="F36" s="49"/>
-      <c r="H36" s="109"/>
+      <c r="H36" s="112"/>
       <c r="I36" s="87" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J36" s="85" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K36" s="85" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L36" s="89" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M36" s="86" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="37" spans="4:14" ht="30" x14ac:dyDescent="0.2">
@@ -3388,22 +3385,22 @@
       <c r="E37" s="7"/>
       <c r="F37" s="49"/>
       <c r="H37" s="78" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I37" s="39" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J37" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="K37" s="38" t="s">
         <v>239</v>
       </c>
-      <c r="K37" s="38" t="s">
+      <c r="L37" s="38" t="s">
         <v>240</v>
       </c>
-      <c r="L37" s="38" t="s">
-        <v>241</v>
-      </c>
       <c r="M37" s="76" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="38" spans="4:14" ht="30" x14ac:dyDescent="0.2">
@@ -3411,19 +3408,19 @@
         <v>53</v>
       </c>
       <c r="I38" s="39" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J38" s="39" t="s">
+        <v>256</v>
+      </c>
+      <c r="K38" s="86" t="s">
+        <v>256</v>
+      </c>
+      <c r="L38" s="90" t="s">
         <v>257</v>
       </c>
-      <c r="K38" s="86" t="s">
-        <v>257</v>
-      </c>
-      <c r="L38" s="90" t="s">
-        <v>258</v>
-      </c>
       <c r="M38" s="76" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="42" spans="4:14" x14ac:dyDescent="0.2">
@@ -3513,12 +3510,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="H4:M4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="H6:M6"/>
     <mergeCell ref="H35:H36"/>
     <mergeCell ref="H16:H17"/>
     <mergeCell ref="H18:H19"/>
@@ -3526,10 +3522,11 @@
     <mergeCell ref="H12:H15"/>
     <mergeCell ref="H27:H29"/>
     <mergeCell ref="H30:H31"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3562,7 +3559,7 @@
         <v>144</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>143</v>
@@ -3575,7 +3572,7 @@
       <c r="B2" s="97"/>
       <c r="C2" s="97"/>
       <c r="D2" s="69" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3591,7 +3588,7 @@
       <c r="B4" s="97"/>
       <c r="C4" s="97"/>
       <c r="D4" s="69" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3607,7 +3604,7 @@
       <c r="B6" s="97"/>
       <c r="C6" s="97"/>
       <c r="D6" s="69" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3623,7 +3620,7 @@
       <c r="B8" s="97"/>
       <c r="C8" s="97"/>
       <c r="D8" s="69" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3631,7 +3628,7 @@
       <c r="B9" s="97"/>
       <c r="C9" s="97"/>
       <c r="D9" s="69" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3639,7 +3636,7 @@
       <c r="B10" s="97"/>
       <c r="C10" s="97"/>
       <c r="D10" s="69" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3655,7 +3652,7 @@
       <c r="B12" s="97"/>
       <c r="C12" s="97"/>
       <c r="D12" s="69" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3671,7 +3668,7 @@
       <c r="B14" s="97"/>
       <c r="C14" s="97"/>
       <c r="D14" s="69" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3679,7 +3676,7 @@
       <c r="B15" s="97"/>
       <c r="C15" s="97"/>
       <c r="D15" s="69" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3687,7 +3684,7 @@
       <c r="B16" s="97"/>
       <c r="C16" s="97"/>
       <c r="D16" s="69" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3695,7 +3692,7 @@
       <c r="B17" s="97"/>
       <c r="C17" s="97"/>
       <c r="D17" s="69" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3713,7 +3710,7 @@
       </c>
       <c r="C19" s="97"/>
       <c r="D19" s="69" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3721,7 +3718,7 @@
       <c r="B20" s="97"/>
       <c r="C20" s="97"/>
       <c r="D20" s="69" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3739,7 +3736,7 @@
       </c>
       <c r="C22" s="97"/>
       <c r="D22" s="69" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3747,7 +3744,7 @@
       <c r="B23" s="97"/>
       <c r="C23" s="97"/>
       <c r="D23" s="69" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3755,7 +3752,7 @@
       <c r="B24" s="97"/>
       <c r="C24" s="97"/>
       <c r="D24" s="69" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3763,7 +3760,7 @@
       <c r="B25" s="97"/>
       <c r="C25" s="97"/>
       <c r="D25" s="69" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3771,7 +3768,7 @@
       <c r="B26" s="97"/>
       <c r="C26" s="97"/>
       <c r="D26" s="69" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3779,7 +3776,7 @@
       <c r="B27" s="97"/>
       <c r="C27" s="97"/>
       <c r="D27" s="69" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3787,7 +3784,7 @@
       <c r="B28" s="97"/>
       <c r="C28" s="97"/>
       <c r="D28" s="69" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3795,7 +3792,7 @@
       <c r="B29" s="97"/>
       <c r="C29" s="97"/>
       <c r="D29" s="105" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3803,7 +3800,7 @@
       <c r="B30" s="97"/>
       <c r="C30" s="97"/>
       <c r="D30" s="105" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3811,7 +3808,7 @@
       <c r="B31" s="97"/>
       <c r="C31" s="97"/>
       <c r="D31" s="105" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3819,7 +3816,7 @@
       <c r="B32" s="97"/>
       <c r="C32" s="97"/>
       <c r="D32" s="105" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -3836,10 +3833,10 @@
         <v>180639</v>
       </c>
       <c r="C34" s="73" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D34" s="69" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="70" customFormat="1" x14ac:dyDescent="0.2">
@@ -4162,7 +4159,7 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="91" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
@@ -4262,7 +4259,7 @@
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="92" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
@@ -4362,7 +4359,7 @@
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="93" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
@@ -4437,7 +4434,7 @@
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" s="93" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
@@ -4447,7 +4444,7 @@
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" s="84" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
@@ -4467,12 +4464,12 @@
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="84" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
@@ -4492,12 +4489,12 @@
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="93" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="93" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
@@ -4512,7 +4509,7 @@
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="93" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
@@ -4522,7 +4519,7 @@
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="84" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
@@ -4542,12 +4539,12 @@
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="84" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="84" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
@@ -4567,12 +4564,12 @@
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" s="93" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="93" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
@@ -4587,7 +4584,7 @@
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" s="93" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
@@ -4597,7 +4594,7 @@
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" s="84" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
@@ -4617,12 +4614,12 @@
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" s="84" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" s="84" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
@@ -4642,12 +4639,12 @@
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" s="93" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" s="93" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -4672,79 +4669,79 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>180</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2" s="1">
         <v>203</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="1">
         <v>208</v>
       </c>
       <c r="C3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" s="1">
         <v>209</v>
       </c>
       <c r="C4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B5" s="1">
         <v>207</v>
       </c>
       <c r="C5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="62" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="62" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B6" s="1">
         <v>210</v>
       </c>
       <c r="C6" s="62" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B7" s="1">
         <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -4755,7 +4752,7 @@
         <v>112</v>
       </c>
       <c r="C8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -4766,40 +4763,40 @@
         <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B10" s="1">
         <v>311</v>
       </c>
       <c r="C10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11" s="1">
         <v>312</v>
       </c>
       <c r="C11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="62" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B12" s="1">
         <v>313</v>
       </c>
       <c r="C12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>